<commit_message>
Created tests for login
</commit_message>
<xml_diff>
--- a/testData/jira_test_data.xlsx
+++ b/testData/jira_test_data.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="login_failed" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -29,15 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">Expected Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCPass123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User profile for User 10</t>
   </si>
   <si>
     <t xml:space="preserve">usernameerror</t>
@@ -154,10 +145,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -179,38 +170,27 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="B2" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="B3" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -218,8 +198,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Általános"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Általános"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Navigate to Issue search, display all
</commit_message>
<xml_diff>
--- a/testData/jira_test_data.xlsx
+++ b/testData/jira_test_data.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login_failed" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="browse_issues" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -38,6 +39,18 @@
   </si>
   <si>
     <t xml:space="preserve">Example123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projects to browse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOUCAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JETI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COALA</t>
   </si>
 </sst>
 </file>
@@ -130,12 +143,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -147,15 +160,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -196,7 +209,55 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
added test data for version creating test cases
</commit_message>
<xml_diff>
--- a/testData/jira_test_data.xlsx
+++ b/testData/jira_test_data.xlsx
@@ -5,10 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="login_failed" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="version_new_success" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="version_new_invalid_name" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="version_new_invalid_date_format" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="version_new_invalid_date_value" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -38,6 +42,87 @@
   </si>
   <si>
     <t xml:space="preserve">Example123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Release date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected outcome – name of version on the top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test version 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/mar/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23/mar/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team Norse Manon Salad created this version for testing purposes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test version 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@~¬¬¬ version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected outcome – attribute present in Add button tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected outcome – xpath of element in which some text is present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test version 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.03.2019.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//form[@id='releases-add__version']/div[@class='releases-add__date-start']/div[@class='error-container']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test version 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.3.2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//form[@id='releases-add__version']/div[@class='releases-add__date-release']/div[@class='error-container']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected outcome – xpath of element in which test version name is the text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test version 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/ma/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//tr[@class='item-state-error-add']/td[@class='versions-table__name']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test version 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22/se/2019</t>
   </si>
 </sst>
 </file>
@@ -47,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -76,6 +161,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -119,12 +209,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -147,7 +241,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -198,8 +292,375 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Általános"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Általános"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="42.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="C3" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="D4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Általános"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Általános"&amp;12Oldal &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="49.09"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="C3" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Általános"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Általános"&amp;12Oldal &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="87.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="D2" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Általános"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Általános"&amp;12Oldal &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="87.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="D2" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Általános"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Általános"&amp;12Oldal &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test if all specified projects has three Issues
</commit_message>
<xml_diff>
--- a/testData/jira_test_data.xlsx
+++ b/testData/jira_test_data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -41,10 +41,16 @@
     <t xml:space="preserve">Example123</t>
   </si>
   <si>
-    <t xml:space="preserve">Projects to browse</t>
+    <t xml:space="preserve">Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Issues required</t>
   </si>
   <si>
     <t xml:space="preserve">TOUCAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
   </si>
   <si>
     <t xml:space="preserve">JETI</t>
@@ -57,8 +63,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -132,12 +139,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -166,9 +177,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -222,36 +234,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>